<commit_message>
Updated documentation to reflect updates to playback file.
</commit_message>
<xml_diff>
--- a/PDWlist_verif.xlsx
+++ b/PDWlist_verif.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GRANTHAM\Documents\python_package_xDW_SMW200A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15EDAA7-A3BC-4208-8315-1CBDEF3D09CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE0CCAA-E9BC-4BFA-BC0E-1DECF6BDE5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{5BD9F2D2-F2EC-4729-BD4E-1CB338A9DADF}"/>
+    <workbookView xWindow="20715" yWindow="0" windowWidth="30990" windowHeight="20985" xr2:uid="{5BD9F2D2-F2EC-4729-BD4E-1CB338A9DADF}"/>
   </bookViews>
   <sheets>
     <sheet name="PDWlist_verif" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Type</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Number of Pulses</t>
   </si>
   <si>
-    <t>:w</t>
-  </si>
-  <si>
     <t>Simple Rectangular x1</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>Tchirp at 1MHz offset x4</t>
   </si>
   <si>
-    <t>Barker at 1MHz offset x4 with marker 1</t>
-  </si>
-  <si>
     <t>Linear chirp at 1MHz offset 10dBm offset x4</t>
   </si>
   <si>
@@ -167,7 +161,13 @@
     <t>Tchirp at 1MHz offset 10dBm 45deg offset x4</t>
   </si>
   <si>
-    <t>Barker at 1MHz offset 10dBm 45deg offset x4</t>
+    <t>Barker at 1MHz offset x4 with external marker 2</t>
+  </si>
+  <si>
+    <t>Barker at 1MHz offset 10dBm 45deg offset x3</t>
+  </si>
+  <si>
+    <t>Barker at 1MHz offset 10dBm 45deg offset x1 with Marker 1</t>
   </si>
 </sst>
 </file>
@@ -538,10 +538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AB61CE-8842-4DFC-A817-49A8D1017CCF}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -708,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -750,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -758,7 +759,7 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B20" si="0">B5+K5*(L5+1)</f>
+        <f t="shared" ref="B6:B21" si="0">B5+K5*(L5+1)</f>
         <v>4.5900000000000003E-2</v>
       </c>
       <c r="C6" t="s">
@@ -795,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -846,7 +847,7 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -891,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -933,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -978,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -1020,16 +1021,16 @@
         <v>4</v>
       </c>
       <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
         <v>1</v>
       </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -1074,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -1116,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -1161,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1212,7 +1213,7 @@
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -1257,7 +1258,7 @@
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -1299,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
@@ -1344,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
@@ -1352,8 +1353,8 @@
         <v>13</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
-        <v>5.2400000000000009E-2</v>
+        <f>B17+K17*(L17+1)</f>
+        <v>5.1900000000000009E-2</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1383,7 +1384,7 @@
         <v>1E-4</v>
       </c>
       <c r="L19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -1395,24 +1396,70 @@
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <f>B18+K18*(L18+1)</f>
+        <v>5.2400000000000009E-2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="E20">
+        <v>1000000</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>45</v>
+      </c>
+      <c r="H20">
+        <v>3.5700000000000001E-6</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1E-4</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>11</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <f t="shared" si="0"/>
-        <v>5.290000000000001E-2</v>
-      </c>
-      <c r="C20" t="s">
+        <v>5.2600000000000008E-2</v>
+      </c>
+      <c r="C21" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J27" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>